<commit_message>
Double Collision Fixed (5 enemy remain)
</commit_message>
<xml_diff>
--- a/BombShootDown/Assets/Templates/Enemies/EnemiesDataList.xlsx
+++ b/BombShootDown/Assets/Templates/Enemies/EnemiesDataList.xlsx
@@ -1388,9 +1388,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC76"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K15" sqref="K15"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E51" sqref="E51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -3037,7 +3037,7 @@
         <v>259</v>
       </c>
       <c r="M44" s="28">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="N44" s="28"/>
       <c r="O44" s="5" t="s">
@@ -3076,7 +3076,7 @@
         <v>259</v>
       </c>
       <c r="M45" s="28">
-        <v>0.02</v>
+        <v>0.03</v>
       </c>
       <c r="N45" s="28"/>
       <c r="O45" s="5" t="s">
@@ -3115,7 +3115,7 @@
         <v>259</v>
       </c>
       <c r="M46" s="28">
-        <v>0.03</v>
+        <v>0.04</v>
       </c>
       <c r="N46" s="28"/>
       <c r="O46" s="5" t="s">
@@ -3175,7 +3175,7 @@
         <v>3</v>
       </c>
       <c r="E48" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F48" s="2" t="s">
         <v>25</v>
@@ -3207,7 +3207,7 @@
         <v>5</v>
       </c>
       <c r="E49" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F49" s="2" t="s">
         <v>26</v>
@@ -3239,7 +3239,7 @@
         <v>8</v>
       </c>
       <c r="E50" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F50" s="2" t="s">
         <v>27</v>
@@ -3271,7 +3271,7 @@
         <v>10</v>
       </c>
       <c r="E51" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F51" s="2" t="s">
         <v>232</v>

</xml_diff>

<commit_message>
Buffer, Debuffer, Core, Carrier Remain
</commit_message>
<xml_diff>
--- a/BombShootDown/Assets/Templates/Enemies/EnemiesDataList.xlsx
+++ b/BombShootDown/Assets/Templates/Enemies/EnemiesDataList.xlsx
@@ -1389,8 +1389,8 @@
   <dimension ref="A1:AC76"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E51" sqref="E51"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N41" sqref="N41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -3028,7 +3028,7 @@
         <v>0</v>
       </c>
       <c r="I44" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="J44" s="4">
         <v>1</v>
@@ -3067,7 +3067,7 @@
         <v>0</v>
       </c>
       <c r="I45" s="4">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="J45" s="4">
         <v>1</v>
@@ -3106,7 +3106,7 @@
         <v>0</v>
       </c>
       <c r="I46" s="4">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="J46" s="4">
         <v>1</v>
@@ -3145,7 +3145,7 @@
         <v>0</v>
       </c>
       <c r="I47" s="4">
-        <v>4</v>
+        <v>25</v>
       </c>
       <c r="J47" s="4">
         <v>1</v>

</xml_diff>

<commit_message>
particle effect bullet done
</commit_message>
<xml_diff>
--- a/BombShootDown/Assets/Templates/Enemies/EnemiesDataList.xlsx
+++ b/BombShootDown/Assets/Templates/Enemies/EnemiesDataList.xlsx
@@ -1398,8 +1398,8 @@
   <dimension ref="A1:AD76"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H73" sqref="H73"/>
+      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K81" sqref="K81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -4083,7 +4083,7 @@
         <v>272</v>
       </c>
       <c r="G67" s="22">
-        <v>1000</v>
+        <v>1500</v>
       </c>
       <c r="H67" s="22">
         <v>2</v>
@@ -4124,7 +4124,7 @@
         <v>273</v>
       </c>
       <c r="G68" s="22">
-        <v>1500</v>
+        <v>2000</v>
       </c>
       <c r="H68" s="22">
         <v>3</v>
@@ -4165,7 +4165,7 @@
         <v>274</v>
       </c>
       <c r="G69" s="22">
-        <v>3000</v>
+        <v>4000</v>
       </c>
       <c r="H69" s="22">
         <v>4</v>
@@ -4206,7 +4206,7 @@
         <v>275</v>
       </c>
       <c r="G70" s="22">
-        <v>4000</v>
+        <v>5000</v>
       </c>
       <c r="H70" s="22">
         <v>5</v>

</xml_diff>

<commit_message>
load screen tips made
</commit_message>
<xml_diff>
--- a/BombShootDown/Assets/Templates/Enemies/EnemiesDataList.xlsx
+++ b/BombShootDown/Assets/Templates/Enemies/EnemiesDataList.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="11840" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="11840"/>
   </bookViews>
   <sheets>
     <sheet name="Basic enemies" sheetId="1" r:id="rId1"/>
@@ -933,9 +933,6 @@
     <t>basic boss</t>
   </si>
   <si>
-    <t>A highly defensive type of bomb geared in protecting its fellow bombs. It shows other effects as well periodically.</t>
-  </si>
-  <si>
     <t>Ultimatebasic</t>
   </si>
   <si>
@@ -1000,6 +997,9 @@
   </si>
   <si>
     <t>mix</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A highly defensive type of bomb geared in protecting its fellow bombs. It shows other abilities as well periodically. </t>
   </si>
 </sst>
 </file>
@@ -1482,9 +1482,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD76"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I59" sqref="I59"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Q71" sqref="Q71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -4362,7 +4362,7 @@
         <v>300</v>
       </c>
       <c r="Q71" s="9" t="s">
-        <v>302</v>
+        <v>324</v>
       </c>
     </row>
     <row r="72" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.5">
@@ -4521,7 +4521,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
@@ -4553,7 +4553,7 @@
         <v>148</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C2" s="24" t="s">
         <v>301</v>
@@ -4591,10 +4591,10 @@
     </row>
     <row r="5" spans="1:5" s="27" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A5" s="17" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C5" s="26"/>
       <c r="D5" s="26"/>
@@ -4602,10 +4602,10 @@
     </row>
     <row r="6" spans="1:5" s="27" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A6" s="17" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C6" s="26"/>
       <c r="D6" s="26"/>
@@ -4613,10 +4613,10 @@
     </row>
     <row r="7" spans="1:5" s="27" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A7" s="17" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B7" s="17" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C7" s="26"/>
       <c r="D7" s="26"/>
@@ -4624,10 +4624,10 @@
     </row>
     <row r="8" spans="1:5" s="27" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A8" s="17" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B8" s="17" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C8" s="26"/>
       <c r="D8" s="26"/>
@@ -4635,10 +4635,10 @@
     </row>
     <row r="9" spans="1:5" s="27" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A9" s="17" t="s">
+        <v>307</v>
+      </c>
+      <c r="B9" s="17" t="s">
         <v>308</v>
-      </c>
-      <c r="B9" s="17" t="s">
-        <v>309</v>
       </c>
       <c r="C9" s="26"/>
       <c r="D9" s="26"/>
@@ -4646,10 +4646,10 @@
     </row>
     <row r="10" spans="1:5" s="29" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A10" s="21" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B10" s="21" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C10" s="28"/>
       <c r="D10" s="28"/>
@@ -4657,10 +4657,10 @@
     </row>
     <row r="11" spans="1:5" s="29" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A11" s="21" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B11" s="21" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C11" s="28"/>
       <c r="D11" s="28"/>
@@ -4668,10 +4668,10 @@
     </row>
     <row r="12" spans="1:5" s="29" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A12" s="21" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B12" s="21" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C12" s="28"/>
       <c r="D12" s="28"/>
@@ -4679,10 +4679,10 @@
     </row>
     <row r="13" spans="1:5" s="29" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A13" s="21" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B13" s="21" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C13" s="28"/>
       <c r="D13" s="28"/>
@@ -4690,10 +4690,10 @@
     </row>
     <row r="14" spans="1:5" s="29" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A14" s="21" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B14" s="21" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C14" s="28"/>
       <c r="D14" s="28"/>
@@ -4701,10 +4701,10 @@
     </row>
     <row r="15" spans="1:5" s="29" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A15" s="21" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B15" s="21" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C15" s="28"/>
       <c r="D15" s="28"/>
@@ -4712,10 +4712,10 @@
     </row>
     <row r="16" spans="1:5" s="29" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A16" s="21" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B16" s="21" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C16" s="28"/>
       <c r="D16" s="28"/>
@@ -4723,10 +4723,10 @@
     </row>
     <row r="17" spans="1:5" s="37" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A17" s="35" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B17" s="35" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C17" s="36"/>
       <c r="D17" s="36"/>

</xml_diff>

<commit_message>
world 2 levels labour nearly done (enemies to be added to level objects)
</commit_message>
<xml_diff>
--- a/BombShootDown/Assets/Templates/Enemies/EnemiesDataList.xlsx
+++ b/BombShootDown/Assets/Templates/Enemies/EnemiesDataList.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="325">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="553" uniqueCount="341">
   <si>
     <t>Name</t>
   </si>
@@ -951,9 +951,6 @@
     <t>[2-30]</t>
   </si>
   <si>
-    <t>new</t>
-  </si>
-  <si>
     <t>mesocarrier</t>
   </si>
   <si>
@@ -996,10 +993,63 @@
     <t>hypercore</t>
   </si>
   <si>
-    <t>mix</t>
-  </si>
-  <si>
     <t xml:space="preserve">A highly defensive type of bomb geared in protecting its fellow bombs. It shows other abilities as well periodically. </t>
+  </si>
+  <si>
+    <t>[2-18]</t>
+  </si>
+  <si>
+    <t>Couplad</t>
+  </si>
+  <si>
+    <t>2 entities are coupled to each other. When 1 dies, it slowly regains hp. If it reaches full hp then it is fully functional again, the only way to kill it is to the kill the other entitiy while one is down. (deals DOT)</t>
+  </si>
+  <si>
+    <t>MaxCouplad</t>
+  </si>
+  <si>
+    <t>same as couplad but now everytime 1 of the entities dies it boost a certain aspect, 1 of the sides boost the speed and other boost damage (DOT increases with each kill as well)</t>
+  </si>
+  <si>
+    <t>Maxima</t>
+  </si>
+  <si>
+    <t>???</t>
+  </si>
+  <si>
+    <t>??? (secret stage boss)</t>
+  </si>
+  <si>
+    <t>2 lives, massive damage, mode change, 1st stage buff &amp; debuffs &amp;reflect dmg 2nd stage DOT &amp; summons (carriers/cores every 40 seconds or smthing) (doesn't move all the way down but deal damage upon each death and if a stage is not killed fast enough it does game ending damage every 4mins or smthing.</t>
+  </si>
+  <si>
+    <t>coupled, maxcouplad</t>
+  </si>
+  <si>
+    <t>Minima</t>
+  </si>
+  <si>
+    <t>small hitbox, buffs speed, moves towards randomm positions in the map, phases in and out of invisibility under 50% health &amp; speed boost.</t>
+  </si>
+  <si>
+    <t>Minima &amp; Gigantodon</t>
+  </si>
+  <si>
+    <t>Gigantodon</t>
+  </si>
+  <si>
+    <t>masssive hp, very wide (pierce to hit stuff behind it), under 20%health recovers hp. Increases your ammo rate but makes it 0 every minute.</t>
+  </si>
+  <si>
+    <t>3 lives, invulnerable during revives. Every stage it picks random abilities among the following, (teleporting movement, spawner, DOT, Buff, Debuff, Taunt &amp; pull, bullets turn invisible, enemies turn invisible periodically) with the numbers chosen as 2,4,6
+during reviving it stops production of bullets &amp; cooldowns
+during its second reviving it summons bunch of other stuff.</t>
+  </si>
+  <si>
+    <t>Ernesto</t>
+  </si>
+  <si>
+    <t>slowly reduces max hp? Possible? If not hit for a time it accrues damage and hits with a burst on next hit. Enemies that detonate on fortress don't deal damage but ernesto holds their damage until it is big and then releases at once.</t>
   </si>
 </sst>
 </file>
@@ -1483,8 +1533,8 @@
   <dimension ref="A1:AD76"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H71" sqref="H71"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L35" sqref="L35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -4362,7 +4412,7 @@
         <v>300</v>
       </c>
       <c r="Q71" s="9" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="72" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.5">
@@ -4519,10 +4569,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="I32" sqref="I32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -4555,9 +4605,7 @@
       <c r="B2" s="20" t="s">
         <v>302</v>
       </c>
-      <c r="C2" s="24" t="s">
-        <v>301</v>
-      </c>
+      <c r="C2" s="24"/>
       <c r="D2" s="24"/>
       <c r="E2" s="24" t="s">
         <v>301</v>
@@ -4570,9 +4618,7 @@
       <c r="B3" s="20" t="s">
         <v>120</v>
       </c>
-      <c r="C3" s="24" t="s">
-        <v>301</v>
-      </c>
+      <c r="C3" s="24"/>
       <c r="D3" s="24"/>
       <c r="E3" s="24" t="s">
         <v>301</v>
@@ -4594,7 +4640,7 @@
         <v>303</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C5" s="26"/>
       <c r="D5" s="26"/>
@@ -4605,7 +4651,7 @@
         <v>305</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C6" s="26"/>
       <c r="D6" s="26"/>
@@ -4613,18 +4659,20 @@
     </row>
     <row r="7" spans="1:5" s="27" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A7" s="17" t="s">
-        <v>304</v>
+        <v>323</v>
       </c>
       <c r="B7" s="17" t="s">
-        <v>311</v>
-      </c>
-      <c r="C7" s="26"/>
+        <v>324</v>
+      </c>
+      <c r="C7" s="26" t="s">
+        <v>325</v>
+      </c>
       <c r="D7" s="26"/>
       <c r="E7" s="26"/>
     </row>
     <row r="8" spans="1:5" s="27" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A8" s="17" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="B8" s="17" t="s">
         <v>310</v>
@@ -4635,43 +4683,47 @@
     </row>
     <row r="9" spans="1:5" s="27" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A9" s="17" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B9" s="17" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="C9" s="26"/>
       <c r="D9" s="26"/>
       <c r="E9" s="26"/>
     </row>
-    <row r="10" spans="1:5" s="29" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A10" s="21" t="s">
-        <v>313</v>
-      </c>
-      <c r="B10" s="21" t="s">
-        <v>308</v>
-      </c>
-      <c r="C10" s="28"/>
-      <c r="D10" s="28"/>
-      <c r="E10" s="28"/>
+    <row r="10" spans="1:5" s="27" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A10" s="17" t="s">
+        <v>307</v>
+      </c>
+      <c r="B10" s="17" t="s">
+        <v>333</v>
+      </c>
+      <c r="C10" s="26" t="s">
+        <v>334</v>
+      </c>
+      <c r="D10" s="26"/>
+      <c r="E10" s="26"/>
     </row>
     <row r="11" spans="1:5" s="29" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A11" s="21" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="B11" s="21" t="s">
-        <v>321</v>
-      </c>
-      <c r="C11" s="28"/>
+        <v>326</v>
+      </c>
+      <c r="C11" s="28" t="s">
+        <v>327</v>
+      </c>
       <c r="D11" s="28"/>
       <c r="E11" s="28"/>
     </row>
     <row r="12" spans="1:5" s="29" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A12" s="21" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="B12" s="21" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="C12" s="28"/>
       <c r="D12" s="28"/>
@@ -4679,10 +4731,10 @@
     </row>
     <row r="13" spans="1:5" s="29" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A13" s="21" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B13" s="21" t="s">
-        <v>308</v>
+        <v>321</v>
       </c>
       <c r="C13" s="28"/>
       <c r="D13" s="28"/>
@@ -4690,21 +4742,23 @@
     </row>
     <row r="14" spans="1:5" s="29" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A14" s="21" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="B14" s="21" t="s">
-        <v>323</v>
-      </c>
-      <c r="C14" s="28"/>
+        <v>336</v>
+      </c>
+      <c r="C14" s="28" t="s">
+        <v>337</v>
+      </c>
       <c r="D14" s="28"/>
       <c r="E14" s="28"/>
     </row>
     <row r="15" spans="1:5" s="29" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A15" s="21" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="B15" s="21" t="s">
-        <v>323</v>
+        <v>332</v>
       </c>
       <c r="C15" s="28"/>
       <c r="D15" s="28"/>
@@ -4712,39 +4766,60 @@
     </row>
     <row r="16" spans="1:5" s="29" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A16" s="21" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="B16" s="21" t="s">
-        <v>308</v>
+        <v>335</v>
       </c>
       <c r="C16" s="28"/>
       <c r="D16" s="28"/>
       <c r="E16" s="28"/>
     </row>
-    <row r="17" spans="1:5" s="37" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A17" s="35" t="s">
-        <v>320</v>
-      </c>
-      <c r="B17" s="35" t="s">
-        <v>308</v>
-      </c>
-      <c r="C17" s="36"/>
-      <c r="D17" s="36"/>
-      <c r="E17" s="36"/>
-    </row>
-    <row r="18" spans="1:5" s="34" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A18" s="32"/>
-      <c r="B18" s="32"/>
-      <c r="C18" s="33"/>
-      <c r="D18" s="33"/>
-      <c r="E18" s="33"/>
+    <row r="17" spans="1:5" s="29" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A17" s="21" t="s">
+        <v>318</v>
+      </c>
+      <c r="B17" s="21" t="s">
+        <v>328</v>
+      </c>
+      <c r="C17" s="28" t="s">
+        <v>331</v>
+      </c>
+      <c r="D17" s="28"/>
+      <c r="E17" s="28"/>
+    </row>
+    <row r="18" spans="1:5" s="37" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A18" s="35" t="s">
+        <v>319</v>
+      </c>
+      <c r="B18" s="35" t="s">
+        <v>339</v>
+      </c>
+      <c r="C18" s="36" t="s">
+        <v>340</v>
+      </c>
+      <c r="D18" s="36"/>
+      <c r="E18" s="36"/>
     </row>
     <row r="19" spans="1:5" s="34" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A19" s="32"/>
-      <c r="B19" s="32"/>
-      <c r="C19" s="33"/>
+      <c r="A19" s="32" t="s">
+        <v>329</v>
+      </c>
+      <c r="B19" s="32" t="s">
+        <v>330</v>
+      </c>
+      <c r="C19" s="33" t="s">
+        <v>338</v>
+      </c>
       <c r="D19" s="33"/>
       <c r="E19" s="33"/>
+    </row>
+    <row r="20" spans="1:5" s="34" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A20" s="32"/>
+      <c r="B20" s="32"/>
+      <c r="C20" s="33"/>
+      <c r="D20" s="33"/>
+      <c r="E20" s="33"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
maxima being fixed rn (ernesto and ??? remain)
</commit_message>
<xml_diff>
--- a/BombShootDown/Assets/Templates/Enemies/EnemiesDataList.xlsx
+++ b/BombShootDown/Assets/Templates/Enemies/EnemiesDataList.xlsx
@@ -1533,8 +1533,8 @@
   <dimension ref="A1:AD76"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L35" sqref="L35"/>
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D57" sqref="D57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -4572,7 +4572,7 @@
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>

</xml_diff>

<commit_message>
endlessUpgraded level script ready for testing and bugs
</commit_message>
<xml_diff>
--- a/BombShootDown/Assets/Templates/Enemies/EnemiesDataList.xlsx
+++ b/BombShootDown/Assets/Templates/Enemies/EnemiesDataList.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="11840"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="11840" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Basic enemies" sheetId="1" r:id="rId1"/>
@@ -1008,9 +1008,6 @@
     <t>MaxCouplad</t>
   </si>
   <si>
-    <t>same as couplad but now everytime 1 of the entities dies it boost a certain aspect, 1 of the sides boost the speed and other boost damage (DOT increases with each kill as well)</t>
-  </si>
-  <si>
     <t>Maxima</t>
   </si>
   <si>
@@ -1035,14 +1032,6 @@
     <t>Gigantodon</t>
   </si>
   <si>
-    <t>masssive hp, very wide (pierce to hit stuff behind it), under 20%health recovers hp. Increases your ammo rate but makes it 0 every minute.</t>
-  </si>
-  <si>
-    <t>3 lives, invulnerable during revives. Every stage it picks random abilities among the following, (teleporting movement, spawner, DOT, Buff, Debuff, Taunt &amp; pull, bullets turn invisible, enemies turn invisible periodically) with the numbers chosen as 2,4,6
-during reviving it stops production of bullets &amp; cooldowns
-during its second reviving it summons bunch of other stuff.</t>
-  </si>
-  <si>
     <t>Ernesto</t>
   </si>
   <si>
@@ -1050,6 +1039,15 @@
   </si>
   <si>
     <t>If not hit for a time it accrues damage and hits with a burst on next hit. Enemies that detonate on fortress don't deal damage but ernesto holds their damage until it is big and then releases at once - these enemies are chosen with certain intervals</t>
+  </si>
+  <si>
+    <t>same as couplad but now everytime 1 of the entities dies it boost each of their effects, 1 of the sides boost the fortress hit damage and other boost DOT.</t>
+  </si>
+  <si>
+    <t>masssive hp, very wide (blocks pierce), under 20%health recovers hp. Increases your ammo rate but makes it 0 every minute.</t>
+  </si>
+  <si>
+    <t>3 lives. Every stage it picks random abilities (abilities are also changed periodically) among the following (9 abilities), (teleporting movement, spawner, DOT, Buff, Debuff, Taunt &amp; pull, enemies turn invisible, vampire heal, block pierce) with the number of abilities at a given time chosen as 2,4,6 depending on the respective number of deaths.</t>
   </si>
 </sst>
 </file>
@@ -1532,9 +1530,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD76"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G4" sqref="G4"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A74" sqref="A74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -4571,8 +4569,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M31" sqref="M31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -4697,10 +4695,10 @@
         <v>307</v>
       </c>
       <c r="B10" s="17" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C10" s="26" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="D10" s="26"/>
       <c r="E10" s="26"/>
@@ -4713,7 +4711,7 @@
         <v>326</v>
       </c>
       <c r="C11" s="28" t="s">
-        <v>327</v>
+        <v>338</v>
       </c>
       <c r="D11" s="28"/>
       <c r="E11" s="28"/>
@@ -4745,10 +4743,10 @@
         <v>315</v>
       </c>
       <c r="B14" s="21" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C14" s="28" t="s">
-        <v>336</v>
+        <v>339</v>
       </c>
       <c r="D14" s="28"/>
       <c r="E14" s="28"/>
@@ -4758,7 +4756,7 @@
         <v>316</v>
       </c>
       <c r="B15" s="21" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C15" s="28"/>
       <c r="D15" s="28"/>
@@ -4769,7 +4767,7 @@
         <v>317</v>
       </c>
       <c r="B16" s="21" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C16" s="28"/>
       <c r="D16" s="28"/>
@@ -4780,10 +4778,10 @@
         <v>318</v>
       </c>
       <c r="B17" s="21" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C17" s="28" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D17" s="28"/>
       <c r="E17" s="28"/>
@@ -4793,23 +4791,23 @@
         <v>319</v>
       </c>
       <c r="B18" s="35" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="C18" s="36" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="D18" s="36"/>
       <c r="E18" s="36"/>
     </row>
     <row r="19" spans="1:5" s="34" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A19" s="32" t="s">
+        <v>328</v>
+      </c>
+      <c r="B19" s="32" t="s">
         <v>329</v>
       </c>
-      <c r="B19" s="32" t="s">
-        <v>330</v>
-      </c>
       <c r="C19" s="33" t="s">
-        <v>337</v>
+        <v>340</v>
       </c>
       <c r="D19" s="33"/>
       <c r="E19" s="33"/>

</xml_diff>

<commit_message>
Added some details to Bosses & levels
</commit_message>
<xml_diff>
--- a/BombShootDown/Assets/Templates/Enemies/EnemiesDataList.xlsx
+++ b/BombShootDown/Assets/Templates/Enemies/EnemiesDataList.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nived\OneDrive\Desktop\Unity Projects Completedish\Project\Shooter thingy\BombShootingGameAndroid\BombShootDown\Assets\Templates\Enemies\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nived\OneDrive\Desktop\Unity Projects Completedish\Project\Shooter thingy\BombShootDown - PreURP\BombShootingGameAndroid\BombShootDown\Assets\Templates\Enemies\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="11840" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="11840"/>
   </bookViews>
   <sheets>
     <sheet name="Basic enemies" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="553" uniqueCount="341">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="588" uniqueCount="358">
   <si>
     <t>Name</t>
   </si>
@@ -1048,6 +1048,57 @@
   </si>
   <si>
     <t>3 lives. Every stage it picks random abilities (abilities are also changed periodically) among the following (9 abilities), (teleporting movement, spawner, DOT, Buff, Debuff, Taunt &amp; pull, enemies turn invisible, vampire heal, block pierce) with the number of abilities at a given time chosen as 2,4,6 depending on the respective number of deaths.</t>
+  </si>
+  <si>
+    <t>MAINBOSSES</t>
+  </si>
+  <si>
+    <t>Gigantadon</t>
+  </si>
+  <si>
+    <t>HiddenBoss</t>
+  </si>
+  <si>
+    <t>A pair of bombs that somehow revivew if not destroyed simultaneously.</t>
+  </si>
+  <si>
+    <t>A dangerous pair of bombs that revive and get strengthened if not destroyed simultaneously.</t>
+  </si>
+  <si>
+    <t>A bomb of truth.</t>
+  </si>
+  <si>
+    <t>The largest bomb to be recorded.</t>
+  </si>
+  <si>
+    <t>A bomb capable of massive destruction.</t>
+  </si>
+  <si>
+    <t>A trickster of a bomb. Difficult to hit.</t>
+  </si>
+  <si>
+    <t>distance to move:</t>
+  </si>
+  <si>
+    <t>0(50)</t>
+  </si>
+  <si>
+    <t>0(60)</t>
+  </si>
+  <si>
+    <t>0(500)</t>
+  </si>
+  <si>
+    <t>0(1000)</t>
+  </si>
+  <si>
+    <t>0/1</t>
+  </si>
+  <si>
+    <t>never comes down.</t>
+  </si>
+  <si>
+    <t>never comes down</t>
   </si>
 </sst>
 </file>
@@ -1165,7 +1216,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1248,6 +1299,11 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1528,11 +1584,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AD76"/>
+  <dimension ref="A1:AD94"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A74" sqref="A74"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G78" sqref="G78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -4559,6 +4615,300 @@
       <c r="O76" s="9"/>
       <c r="Q76" s="9"/>
     </row>
+    <row r="77" spans="1:17" x14ac:dyDescent="0.5">
+      <c r="A77" s="5" t="s">
+        <v>341</v>
+      </c>
+      <c r="B77" s="5" t="s">
+        <v>324</v>
+      </c>
+      <c r="F77" s="5" t="s">
+        <v>351</v>
+      </c>
+      <c r="G77" s="5">
+        <v>1000</v>
+      </c>
+      <c r="H77" s="5">
+        <v>2</v>
+      </c>
+      <c r="I77" s="5">
+        <v>200</v>
+      </c>
+      <c r="J77" s="5">
+        <v>0</v>
+      </c>
+      <c r="K77" s="5">
+        <v>2</v>
+      </c>
+      <c r="M77" s="38" t="s">
+        <v>350</v>
+      </c>
+      <c r="N77" s="38"/>
+      <c r="O77" s="39" t="s">
+        <v>325</v>
+      </c>
+      <c r="Q77" s="6" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="78" spans="1:17" x14ac:dyDescent="0.5">
+      <c r="B78" s="5" t="s">
+        <v>326</v>
+      </c>
+      <c r="F78" s="5" t="s">
+        <v>352</v>
+      </c>
+      <c r="G78" s="5">
+        <v>1500</v>
+      </c>
+      <c r="H78" s="5">
+        <v>4</v>
+      </c>
+      <c r="I78" s="5">
+        <v>300</v>
+      </c>
+      <c r="J78" s="5">
+        <v>0</v>
+      </c>
+      <c r="K78" s="5">
+        <v>2</v>
+      </c>
+      <c r="M78" s="38" t="s">
+        <v>350</v>
+      </c>
+      <c r="N78" s="38"/>
+      <c r="O78" s="39" t="s">
+        <v>338</v>
+      </c>
+      <c r="Q78" s="6" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="79" spans="1:17" x14ac:dyDescent="0.5">
+      <c r="B79" s="5" t="s">
+        <v>332</v>
+      </c>
+      <c r="D79" s="5">
+        <v>120</v>
+      </c>
+      <c r="F79" s="5" t="s">
+        <v>271</v>
+      </c>
+      <c r="G79" s="5">
+        <v>3000</v>
+      </c>
+      <c r="H79" s="5">
+        <v>2</v>
+      </c>
+      <c r="I79" s="5">
+        <v>100</v>
+      </c>
+      <c r="J79" s="5">
+        <v>0</v>
+      </c>
+      <c r="K79" s="5">
+        <v>2</v>
+      </c>
+      <c r="M79" s="38" t="s">
+        <v>350</v>
+      </c>
+      <c r="N79" s="38"/>
+      <c r="O79" s="39" t="s">
+        <v>336</v>
+      </c>
+      <c r="Q79" s="6" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="80" spans="1:17" x14ac:dyDescent="0.5">
+      <c r="B80" s="5" t="s">
+        <v>327</v>
+      </c>
+      <c r="D80" s="5">
+        <v>300</v>
+      </c>
+      <c r="F80" s="5" t="s">
+        <v>353</v>
+      </c>
+      <c r="G80" s="5">
+        <v>9000</v>
+      </c>
+      <c r="H80" s="5">
+        <v>6</v>
+      </c>
+      <c r="I80" s="5">
+        <v>1000</v>
+      </c>
+      <c r="J80" s="5">
+        <v>0</v>
+      </c>
+      <c r="K80" s="5">
+        <v>2</v>
+      </c>
+      <c r="M80" s="38" t="s">
+        <v>357</v>
+      </c>
+      <c r="N80" s="38"/>
+      <c r="O80" s="39" t="s">
+        <v>330</v>
+      </c>
+      <c r="Q80" s="6" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="81" spans="2:17" x14ac:dyDescent="0.5">
+      <c r="B81" s="5" t="s">
+        <v>342</v>
+      </c>
+      <c r="D81" s="5">
+        <v>300</v>
+      </c>
+      <c r="F81" s="5" t="s">
+        <v>354</v>
+      </c>
+      <c r="G81" s="5">
+        <v>25000</v>
+      </c>
+      <c r="H81" s="5">
+        <v>8</v>
+      </c>
+      <c r="I81" s="5">
+        <v>1000000</v>
+      </c>
+      <c r="J81" s="5">
+        <v>0</v>
+      </c>
+      <c r="K81" s="5">
+        <v>2</v>
+      </c>
+      <c r="M81" s="38"/>
+      <c r="N81" s="38"/>
+      <c r="O81" s="39" t="s">
+        <v>339</v>
+      </c>
+      <c r="Q81" s="6" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="82" spans="2:17" x14ac:dyDescent="0.5">
+      <c r="B82" s="5" t="s">
+        <v>335</v>
+      </c>
+      <c r="D82" s="5">
+        <v>300</v>
+      </c>
+      <c r="F82" s="5" t="s">
+        <v>271</v>
+      </c>
+      <c r="G82" s="5">
+        <v>20000</v>
+      </c>
+      <c r="H82" s="5">
+        <v>1</v>
+      </c>
+      <c r="I82" s="5">
+        <v>900</v>
+      </c>
+      <c r="J82" s="5">
+        <v>0</v>
+      </c>
+      <c r="K82" s="5">
+        <v>2</v>
+      </c>
+      <c r="M82" s="38"/>
+      <c r="N82" s="38"/>
+      <c r="O82" s="39" t="s">
+        <v>337</v>
+      </c>
+      <c r="Q82" s="6" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="83" spans="2:17" x14ac:dyDescent="0.5">
+      <c r="B83" s="5" t="s">
+        <v>343</v>
+      </c>
+      <c r="D83" s="5">
+        <v>300</v>
+      </c>
+      <c r="F83" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G83" s="5">
+        <v>8000</v>
+      </c>
+      <c r="H83" s="5">
+        <v>5</v>
+      </c>
+      <c r="I83" s="5">
+        <v>10000</v>
+      </c>
+      <c r="J83" s="5" t="s">
+        <v>355</v>
+      </c>
+      <c r="K83" s="5">
+        <v>2</v>
+      </c>
+      <c r="M83" s="39" t="s">
+        <v>356</v>
+      </c>
+      <c r="N83" s="38"/>
+      <c r="O83" s="39" t="s">
+        <v>340</v>
+      </c>
+      <c r="Q83" s="6" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="84" spans="2:17" x14ac:dyDescent="0.5">
+      <c r="M84" s="39"/>
+      <c r="N84" s="38"/>
+      <c r="O84" s="40"/>
+    </row>
+    <row r="85" spans="2:17" x14ac:dyDescent="0.5">
+      <c r="N85" s="38"/>
+      <c r="O85" s="40"/>
+    </row>
+    <row r="86" spans="2:17" x14ac:dyDescent="0.5">
+      <c r="N86" s="38"/>
+      <c r="O86" s="40"/>
+    </row>
+    <row r="87" spans="2:17" x14ac:dyDescent="0.5">
+      <c r="M87" s="39"/>
+      <c r="N87" s="38"/>
+      <c r="O87" s="40"/>
+    </row>
+    <row r="88" spans="2:17" x14ac:dyDescent="0.5">
+      <c r="M88" s="39"/>
+      <c r="N88" s="38"/>
+      <c r="O88" s="40"/>
+    </row>
+    <row r="89" spans="2:17" x14ac:dyDescent="0.5">
+      <c r="N89" s="38"/>
+      <c r="O89" s="40"/>
+    </row>
+    <row r="90" spans="2:17" x14ac:dyDescent="0.5">
+      <c r="M90" s="39"/>
+      <c r="N90" s="38"/>
+      <c r="O90" s="40"/>
+    </row>
+    <row r="91" spans="2:17" x14ac:dyDescent="0.5">
+      <c r="M91" s="39"/>
+      <c r="N91" s="38"/>
+      <c r="O91" s="40"/>
+    </row>
+    <row r="92" spans="2:17" x14ac:dyDescent="0.5">
+      <c r="N92" s="38"/>
+      <c r="O92" s="40"/>
+    </row>
+    <row r="93" spans="2:17" x14ac:dyDescent="0.5">
+      <c r="N93" s="38"/>
+      <c r="O93" s="40"/>
+    </row>
+    <row r="94" spans="2:17" x14ac:dyDescent="0.5">
+      <c r="N94" s="38"/>
+      <c r="O94" s="40"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -4569,8 +4919,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M31" sqref="M31"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7:C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>

</xml_diff>

<commit_message>
level basics set up (coding levels are only remaining)
</commit_message>
<xml_diff>
--- a/BombShootDown/Assets/Templates/Enemies/EnemiesDataList.xlsx
+++ b/BombShootDown/Assets/Templates/Enemies/EnemiesDataList.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="588" uniqueCount="358">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="592" uniqueCount="361">
   <si>
     <t>Name</t>
   </si>
@@ -1099,6 +1099,15 @@
   </si>
   <si>
     <t>never comes down</t>
+  </si>
+  <si>
+    <t>130,80</t>
+  </si>
+  <si>
+    <t>10,5</t>
+  </si>
+  <si>
+    <t>80,50</t>
   </si>
 </sst>
 </file>
@@ -1121,7 +1130,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1188,6 +1197,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF9999FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -1216,7 +1231,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1259,7 +1274,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1304,12 +1318,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF9999FF"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1587,8 +1617,8 @@
   <dimension ref="A1:AD94"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G78" sqref="G78"/>
+      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M52" sqref="M52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -4601,313 +4631,347 @@
         <v>193</v>
       </c>
     </row>
-    <row r="75" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="L75" s="16"/>
-      <c r="M75" s="16"/>
-      <c r="N75" s="16"/>
-      <c r="O75" s="9"/>
-      <c r="Q75" s="9"/>
-    </row>
-    <row r="76" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="L76" s="16"/>
-      <c r="M76" s="16"/>
-      <c r="N76" s="16"/>
-      <c r="O76" s="9"/>
-      <c r="Q76" s="9"/>
-    </row>
-    <row r="77" spans="1:17" x14ac:dyDescent="0.5">
-      <c r="A77" s="5" t="s">
+    <row r="75" spans="1:17" s="40" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="L75" s="37"/>
+      <c r="M75" s="37"/>
+      <c r="N75" s="37"/>
+      <c r="O75" s="39"/>
+      <c r="Q75" s="39"/>
+    </row>
+    <row r="76" spans="1:17" s="40" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="L76" s="37"/>
+      <c r="M76" s="37"/>
+      <c r="N76" s="37"/>
+      <c r="O76" s="39"/>
+      <c r="Q76" s="39"/>
+    </row>
+    <row r="77" spans="1:17" s="41" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A77" s="41" t="s">
         <v>341</v>
       </c>
-      <c r="B77" s="5" t="s">
+      <c r="B77" s="41" t="s">
         <v>324</v>
       </c>
-      <c r="F77" s="5" t="s">
+      <c r="D77" s="41" t="s">
+        <v>358</v>
+      </c>
+      <c r="E77" s="41" t="s">
+        <v>359</v>
+      </c>
+      <c r="F77" s="41" t="s">
         <v>351</v>
       </c>
-      <c r="G77" s="5">
+      <c r="G77" s="41">
         <v>1000</v>
       </c>
-      <c r="H77" s="5">
+      <c r="H77" s="41">
         <v>2</v>
       </c>
-      <c r="I77" s="5">
+      <c r="I77" s="41">
         <v>200</v>
       </c>
-      <c r="J77" s="5">
-        <v>0</v>
-      </c>
-      <c r="K77" s="5">
+      <c r="J77" s="41">
+        <v>0</v>
+      </c>
+      <c r="K77" s="41">
         <v>2</v>
       </c>
-      <c r="M77" s="38" t="s">
+      <c r="L77" s="42"/>
+      <c r="M77" s="42" t="s">
         <v>350</v>
       </c>
-      <c r="N77" s="38"/>
-      <c r="O77" s="39" t="s">
+      <c r="N77" s="42"/>
+      <c r="O77" s="43" t="s">
         <v>325</v>
       </c>
-      <c r="Q77" s="6" t="s">
+      <c r="Q77" s="44" t="s">
         <v>344</v>
       </c>
     </row>
-    <row r="78" spans="1:17" x14ac:dyDescent="0.5">
-      <c r="B78" s="5" t="s">
+    <row r="78" spans="1:17" s="41" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="B78" s="41" t="s">
         <v>326</v>
       </c>
-      <c r="F78" s="5" t="s">
+      <c r="D78" s="41" t="s">
+        <v>360</v>
+      </c>
+      <c r="E78" s="41" t="s">
+        <v>359</v>
+      </c>
+      <c r="F78" s="41" t="s">
         <v>352</v>
       </c>
-      <c r="G78" s="5">
+      <c r="G78" s="41">
         <v>1500</v>
       </c>
-      <c r="H78" s="5">
+      <c r="H78" s="41">
         <v>4</v>
       </c>
-      <c r="I78" s="5">
+      <c r="I78" s="41">
         <v>300</v>
       </c>
-      <c r="J78" s="5">
-        <v>0</v>
-      </c>
-      <c r="K78" s="5">
+      <c r="J78" s="41">
+        <v>0</v>
+      </c>
+      <c r="K78" s="41">
         <v>2</v>
       </c>
-      <c r="M78" s="38" t="s">
+      <c r="L78" s="42"/>
+      <c r="M78" s="42" t="s">
         <v>350</v>
       </c>
-      <c r="N78" s="38"/>
-      <c r="O78" s="39" t="s">
+      <c r="N78" s="42"/>
+      <c r="O78" s="43" t="s">
         <v>338</v>
       </c>
-      <c r="Q78" s="6" t="s">
+      <c r="Q78" s="44" t="s">
         <v>345</v>
       </c>
     </row>
-    <row r="79" spans="1:17" x14ac:dyDescent="0.5">
-      <c r="B79" s="5" t="s">
+    <row r="79" spans="1:17" s="41" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="B79" s="41" t="s">
         <v>332</v>
       </c>
-      <c r="D79" s="5">
+      <c r="D79" s="41">
         <v>120</v>
       </c>
-      <c r="F79" s="5" t="s">
+      <c r="E79" s="41">
+        <v>4</v>
+      </c>
+      <c r="F79" s="41" t="s">
         <v>271</v>
       </c>
-      <c r="G79" s="5">
+      <c r="G79" s="41">
         <v>3000</v>
       </c>
-      <c r="H79" s="5">
+      <c r="H79" s="41">
         <v>2</v>
       </c>
-      <c r="I79" s="5">
+      <c r="I79" s="41">
         <v>100</v>
       </c>
-      <c r="J79" s="5">
-        <v>0</v>
-      </c>
-      <c r="K79" s="5">
+      <c r="J79" s="41">
+        <v>0</v>
+      </c>
+      <c r="K79" s="41">
         <v>2</v>
       </c>
-      <c r="M79" s="38" t="s">
+      <c r="L79" s="42"/>
+      <c r="M79" s="42" t="s">
         <v>350</v>
       </c>
-      <c r="N79" s="38"/>
-      <c r="O79" s="39" t="s">
+      <c r="N79" s="42"/>
+      <c r="O79" s="43" t="s">
         <v>336</v>
       </c>
-      <c r="Q79" s="6" t="s">
+      <c r="Q79" s="44" t="s">
         <v>349</v>
       </c>
     </row>
-    <row r="80" spans="1:17" x14ac:dyDescent="0.5">
-      <c r="B80" s="5" t="s">
+    <row r="80" spans="1:17" s="41" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="B80" s="41" t="s">
         <v>327</v>
       </c>
-      <c r="D80" s="5">
+      <c r="D80" s="41">
         <v>300</v>
       </c>
-      <c r="F80" s="5" t="s">
+      <c r="E80" s="41">
+        <v>2</v>
+      </c>
+      <c r="F80" s="41" t="s">
         <v>353</v>
       </c>
-      <c r="G80" s="5">
+      <c r="G80" s="41">
         <v>9000</v>
       </c>
-      <c r="H80" s="5">
+      <c r="H80" s="41">
         <v>6</v>
       </c>
-      <c r="I80" s="5">
+      <c r="I80" s="41">
         <v>1000</v>
       </c>
-      <c r="J80" s="5">
-        <v>0</v>
-      </c>
-      <c r="K80" s="5">
+      <c r="J80" s="41">
+        <v>0</v>
+      </c>
+      <c r="K80" s="41">
         <v>2</v>
       </c>
-      <c r="M80" s="38" t="s">
+      <c r="L80" s="42"/>
+      <c r="M80" s="42" t="s">
         <v>357</v>
       </c>
-      <c r="N80" s="38"/>
-      <c r="O80" s="39" t="s">
+      <c r="N80" s="42"/>
+      <c r="O80" s="43" t="s">
         <v>330</v>
       </c>
-      <c r="Q80" s="6" t="s">
+      <c r="Q80" s="44" t="s">
         <v>348</v>
       </c>
     </row>
-    <row r="81" spans="2:17" x14ac:dyDescent="0.5">
-      <c r="B81" s="5" t="s">
+    <row r="81" spans="2:17" s="41" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="B81" s="41" t="s">
         <v>342</v>
       </c>
-      <c r="D81" s="5">
+      <c r="D81" s="41">
         <v>300</v>
       </c>
-      <c r="F81" s="5" t="s">
+      <c r="E81" s="41">
+        <v>0.05</v>
+      </c>
+      <c r="F81" s="41" t="s">
         <v>354</v>
       </c>
-      <c r="G81" s="5">
+      <c r="G81" s="41">
         <v>25000</v>
       </c>
-      <c r="H81" s="5">
+      <c r="H81" s="41">
         <v>8</v>
       </c>
-      <c r="I81" s="5">
+      <c r="I81" s="41">
         <v>1000000</v>
       </c>
-      <c r="J81" s="5">
-        <v>0</v>
-      </c>
-      <c r="K81" s="5">
+      <c r="J81" s="41">
+        <v>0</v>
+      </c>
+      <c r="K81" s="41">
         <v>2</v>
       </c>
-      <c r="M81" s="38"/>
-      <c r="N81" s="38"/>
-      <c r="O81" s="39" t="s">
+      <c r="L81" s="42"/>
+      <c r="M81" s="42"/>
+      <c r="N81" s="42"/>
+      <c r="O81" s="43" t="s">
         <v>339</v>
       </c>
-      <c r="Q81" s="6" t="s">
+      <c r="Q81" s="44" t="s">
         <v>347</v>
       </c>
     </row>
-    <row r="82" spans="2:17" x14ac:dyDescent="0.5">
-      <c r="B82" s="5" t="s">
+    <row r="82" spans="2:17" s="41" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="B82" s="41" t="s">
         <v>335</v>
       </c>
-      <c r="D82" s="5">
+      <c r="D82" s="41">
         <v>300</v>
       </c>
-      <c r="F82" s="5" t="s">
+      <c r="E82" s="41">
+        <v>0</v>
+      </c>
+      <c r="F82" s="41" t="s">
         <v>271</v>
       </c>
-      <c r="G82" s="5">
+      <c r="G82" s="41">
         <v>20000</v>
       </c>
-      <c r="H82" s="5">
+      <c r="H82" s="41">
         <v>1</v>
       </c>
-      <c r="I82" s="5">
+      <c r="I82" s="41">
         <v>900</v>
       </c>
-      <c r="J82" s="5">
-        <v>0</v>
-      </c>
-      <c r="K82" s="5">
+      <c r="J82" s="41">
+        <v>0</v>
+      </c>
+      <c r="K82" s="41">
         <v>2</v>
       </c>
-      <c r="M82" s="38"/>
-      <c r="N82" s="38"/>
-      <c r="O82" s="39" t="s">
+      <c r="L82" s="42"/>
+      <c r="M82" s="42"/>
+      <c r="N82" s="42"/>
+      <c r="O82" s="43" t="s">
         <v>337</v>
       </c>
-      <c r="Q82" s="6" t="s">
+      <c r="Q82" s="44" t="s">
         <v>346</v>
       </c>
     </row>
-    <row r="83" spans="2:17" x14ac:dyDescent="0.5">
-      <c r="B83" s="5" t="s">
+    <row r="83" spans="2:17" s="41" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="B83" s="41" t="s">
         <v>343</v>
       </c>
-      <c r="D83" s="5">
+      <c r="D83" s="41">
         <v>300</v>
       </c>
-      <c r="F83" s="5" t="s">
+      <c r="E83" s="41">
+        <v>3</v>
+      </c>
+      <c r="F83" s="41" t="s">
         <v>29</v>
       </c>
-      <c r="G83" s="5">
+      <c r="G83" s="41">
         <v>8000</v>
       </c>
-      <c r="H83" s="5">
+      <c r="H83" s="41">
         <v>5</v>
       </c>
-      <c r="I83" s="5">
+      <c r="I83" s="41">
         <v>10000</v>
       </c>
-      <c r="J83" s="5" t="s">
+      <c r="J83" s="41" t="s">
         <v>355</v>
       </c>
-      <c r="K83" s="5">
+      <c r="K83" s="41">
         <v>2</v>
       </c>
-      <c r="M83" s="39" t="s">
+      <c r="L83" s="42"/>
+      <c r="M83" s="43" t="s">
         <v>356</v>
       </c>
-      <c r="N83" s="38"/>
-      <c r="O83" s="39" t="s">
+      <c r="N83" s="42"/>
+      <c r="O83" s="43" t="s">
         <v>340</v>
       </c>
-      <c r="Q83" s="6" t="s">
+      <c r="Q83" s="44" t="s">
         <v>328</v>
       </c>
     </row>
     <row r="84" spans="2:17" x14ac:dyDescent="0.5">
-      <c r="M84" s="39"/>
-      <c r="N84" s="38"/>
-      <c r="O84" s="40"/>
+      <c r="M84" s="38"/>
+      <c r="N84" s="37"/>
+      <c r="O84" s="39"/>
     </row>
     <row r="85" spans="2:17" x14ac:dyDescent="0.5">
-      <c r="N85" s="38"/>
-      <c r="O85" s="40"/>
+      <c r="N85" s="37"/>
+      <c r="O85" s="39"/>
     </row>
     <row r="86" spans="2:17" x14ac:dyDescent="0.5">
-      <c r="N86" s="38"/>
-      <c r="O86" s="40"/>
+      <c r="N86" s="37"/>
+      <c r="O86" s="39"/>
     </row>
     <row r="87" spans="2:17" x14ac:dyDescent="0.5">
-      <c r="M87" s="39"/>
-      <c r="N87" s="38"/>
-      <c r="O87" s="40"/>
+      <c r="M87" s="38"/>
+      <c r="N87" s="37"/>
+      <c r="O87" s="39"/>
     </row>
     <row r="88" spans="2:17" x14ac:dyDescent="0.5">
-      <c r="M88" s="39"/>
-      <c r="N88" s="38"/>
-      <c r="O88" s="40"/>
+      <c r="M88" s="38"/>
+      <c r="N88" s="37"/>
+      <c r="O88" s="39"/>
     </row>
     <row r="89" spans="2:17" x14ac:dyDescent="0.5">
-      <c r="N89" s="38"/>
-      <c r="O89" s="40"/>
+      <c r="N89" s="37"/>
+      <c r="O89" s="39"/>
     </row>
     <row r="90" spans="2:17" x14ac:dyDescent="0.5">
-      <c r="M90" s="39"/>
-      <c r="N90" s="38"/>
-      <c r="O90" s="40"/>
+      <c r="M90" s="38"/>
+      <c r="N90" s="37"/>
+      <c r="O90" s="39"/>
     </row>
     <row r="91" spans="2:17" x14ac:dyDescent="0.5">
-      <c r="M91" s="39"/>
-      <c r="N91" s="38"/>
-      <c r="O91" s="40"/>
+      <c r="M91" s="38"/>
+      <c r="N91" s="37"/>
+      <c r="O91" s="39"/>
     </row>
     <row r="92" spans="2:17" x14ac:dyDescent="0.5">
-      <c r="N92" s="38"/>
-      <c r="O92" s="40"/>
+      <c r="N92" s="37"/>
+      <c r="O92" s="39"/>
     </row>
     <row r="93" spans="2:17" x14ac:dyDescent="0.5">
-      <c r="N93" s="38"/>
-      <c r="O93" s="40"/>
+      <c r="N93" s="37"/>
+      <c r="O93" s="39"/>
     </row>
     <row r="94" spans="2:17" x14ac:dyDescent="0.5">
-      <c r="N94" s="38"/>
-      <c r="O94" s="40"/>
+      <c r="N94" s="37"/>
+      <c r="O94" s="39"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4925,249 +4989,249 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="8.9375" style="22"/>
-    <col min="2" max="2" width="21.64453125" style="22" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="12.8203125" style="30" customWidth="1"/>
-    <col min="6" max="16384" width="8.9375" style="31"/>
+    <col min="1" max="1" width="8.9375" style="21"/>
+    <col min="2" max="2" width="21.64453125" style="21" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="12.8203125" style="29" customWidth="1"/>
+    <col min="6" max="16384" width="8.9375" style="30"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="18" t="s">
+    <row r="1" spans="1:5" s="17" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A1" s="17" t="s">
         <v>147</v>
       </c>
-      <c r="B1" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="23" t="s">
+      <c r="B1" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23" t="s">
+      <c r="D1" s="22"/>
+      <c r="E1" s="22" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="25" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A2" s="19" t="s">
+    <row r="2" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A2" s="18" t="s">
         <v>148</v>
       </c>
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="19" t="s">
         <v>302</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24" t="s">
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="25" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A3" s="20" t="s">
+    <row r="3" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A3" s="19" t="s">
         <v>149</v>
       </c>
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="19" t="s">
         <v>120</v>
       </c>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24" t="s">
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="25" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A4" s="20" t="s">
+    <row r="4" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A4" s="19" t="s">
         <v>150</v>
       </c>
-      <c r="B4" s="20" t="s">
+      <c r="B4" s="19" t="s">
         <v>124</v>
       </c>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-    </row>
-    <row r="5" spans="1:5" s="27" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A5" s="17" t="s">
+      <c r="C4" s="23"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
+    </row>
+    <row r="5" spans="1:5" s="26" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A5" s="16" t="s">
         <v>303</v>
       </c>
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="16" t="s">
         <v>311</v>
       </c>
-      <c r="C5" s="26"/>
-      <c r="D5" s="26"/>
-      <c r="E5" s="26"/>
-    </row>
-    <row r="6" spans="1:5" s="27" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A6" s="17" t="s">
+      <c r="C5" s="25"/>
+      <c r="D5" s="25"/>
+      <c r="E5" s="25"/>
+    </row>
+    <row r="6" spans="1:5" s="26" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A6" s="16" t="s">
         <v>305</v>
       </c>
-      <c r="B6" s="17" t="s">
+      <c r="B6" s="16" t="s">
         <v>308</v>
       </c>
-      <c r="C6" s="26"/>
-      <c r="D6" s="26"/>
-      <c r="E6" s="26"/>
-    </row>
-    <row r="7" spans="1:5" s="27" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A7" s="17" t="s">
+      <c r="C6" s="25"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="25"/>
+    </row>
+    <row r="7" spans="1:5" s="26" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A7" s="16" t="s">
         <v>323</v>
       </c>
-      <c r="B7" s="17" t="s">
+      <c r="B7" s="16" t="s">
         <v>324</v>
       </c>
-      <c r="C7" s="26" t="s">
+      <c r="C7" s="25" t="s">
         <v>325</v>
       </c>
-      <c r="D7" s="26"/>
-      <c r="E7" s="26"/>
-    </row>
-    <row r="8" spans="1:5" s="27" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A8" s="17" t="s">
+      <c r="D7" s="25"/>
+      <c r="E7" s="25"/>
+    </row>
+    <row r="8" spans="1:5" s="26" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A8" s="16" t="s">
         <v>304</v>
       </c>
-      <c r="B8" s="17" t="s">
+      <c r="B8" s="16" t="s">
         <v>310</v>
       </c>
-      <c r="C8" s="26"/>
-      <c r="D8" s="26"/>
-      <c r="E8" s="26"/>
-    </row>
-    <row r="9" spans="1:5" s="27" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A9" s="17" t="s">
+      <c r="C8" s="25"/>
+      <c r="D8" s="25"/>
+      <c r="E8" s="25"/>
+    </row>
+    <row r="9" spans="1:5" s="26" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A9" s="16" t="s">
         <v>306</v>
       </c>
-      <c r="B9" s="17" t="s">
+      <c r="B9" s="16" t="s">
         <v>309</v>
       </c>
-      <c r="C9" s="26"/>
-      <c r="D9" s="26"/>
-      <c r="E9" s="26"/>
-    </row>
-    <row r="10" spans="1:5" s="27" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A10" s="17" t="s">
+      <c r="C9" s="25"/>
+      <c r="D9" s="25"/>
+      <c r="E9" s="25"/>
+    </row>
+    <row r="10" spans="1:5" s="26" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A10" s="16" t="s">
         <v>307</v>
       </c>
-      <c r="B10" s="17" t="s">
+      <c r="B10" s="16" t="s">
         <v>332</v>
       </c>
-      <c r="C10" s="26" t="s">
+      <c r="C10" s="25" t="s">
         <v>336</v>
       </c>
-      <c r="D10" s="26"/>
-      <c r="E10" s="26"/>
-    </row>
-    <row r="11" spans="1:5" s="29" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A11" s="21" t="s">
+      <c r="D10" s="25"/>
+      <c r="E10" s="25"/>
+    </row>
+    <row r="11" spans="1:5" s="28" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A11" s="20" t="s">
         <v>312</v>
       </c>
-      <c r="B11" s="21" t="s">
+      <c r="B11" s="20" t="s">
         <v>326</v>
       </c>
-      <c r="C11" s="28" t="s">
+      <c r="C11" s="27" t="s">
         <v>338</v>
       </c>
-      <c r="D11" s="28"/>
-      <c r="E11" s="28"/>
-    </row>
-    <row r="12" spans="1:5" s="29" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A12" s="21" t="s">
+      <c r="D11" s="27"/>
+      <c r="E11" s="27"/>
+    </row>
+    <row r="12" spans="1:5" s="28" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A12" s="20" t="s">
         <v>313</v>
       </c>
-      <c r="B12" s="21" t="s">
+      <c r="B12" s="20" t="s">
         <v>320</v>
       </c>
-      <c r="C12" s="28"/>
-      <c r="D12" s="28"/>
-      <c r="E12" s="28"/>
-    </row>
-    <row r="13" spans="1:5" s="29" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A13" s="21" t="s">
+      <c r="C12" s="27"/>
+      <c r="D12" s="27"/>
+      <c r="E12" s="27"/>
+    </row>
+    <row r="13" spans="1:5" s="28" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A13" s="20" t="s">
         <v>314</v>
       </c>
-      <c r="B13" s="21" t="s">
+      <c r="B13" s="20" t="s">
         <v>321</v>
       </c>
-      <c r="C13" s="28"/>
-      <c r="D13" s="28"/>
-      <c r="E13" s="28"/>
-    </row>
-    <row r="14" spans="1:5" s="29" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A14" s="21" t="s">
+      <c r="C13" s="27"/>
+      <c r="D13" s="27"/>
+      <c r="E13" s="27"/>
+    </row>
+    <row r="14" spans="1:5" s="28" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A14" s="20" t="s">
         <v>315</v>
       </c>
-      <c r="B14" s="21" t="s">
+      <c r="B14" s="20" t="s">
         <v>334</v>
       </c>
-      <c r="C14" s="28" t="s">
+      <c r="C14" s="27" t="s">
         <v>339</v>
       </c>
-      <c r="D14" s="28"/>
-      <c r="E14" s="28"/>
-    </row>
-    <row r="15" spans="1:5" s="29" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A15" s="21" t="s">
+      <c r="D14" s="27"/>
+      <c r="E14" s="27"/>
+    </row>
+    <row r="15" spans="1:5" s="28" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A15" s="20" t="s">
         <v>316</v>
       </c>
-      <c r="B15" s="21" t="s">
+      <c r="B15" s="20" t="s">
         <v>331</v>
       </c>
-      <c r="C15" s="28"/>
-      <c r="D15" s="28"/>
-      <c r="E15" s="28"/>
-    </row>
-    <row r="16" spans="1:5" s="29" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A16" s="21" t="s">
+      <c r="C15" s="27"/>
+      <c r="D15" s="27"/>
+      <c r="E15" s="27"/>
+    </row>
+    <row r="16" spans="1:5" s="28" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A16" s="20" t="s">
         <v>317</v>
       </c>
-      <c r="B16" s="21" t="s">
+      <c r="B16" s="20" t="s">
         <v>333</v>
       </c>
-      <c r="C16" s="28"/>
-      <c r="D16" s="28"/>
-      <c r="E16" s="28"/>
-    </row>
-    <row r="17" spans="1:5" s="29" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A17" s="21" t="s">
+      <c r="C16" s="27"/>
+      <c r="D16" s="27"/>
+      <c r="E16" s="27"/>
+    </row>
+    <row r="17" spans="1:5" s="28" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A17" s="20" t="s">
         <v>318</v>
       </c>
-      <c r="B17" s="21" t="s">
+      <c r="B17" s="20" t="s">
         <v>327</v>
       </c>
-      <c r="C17" s="28" t="s">
+      <c r="C17" s="27" t="s">
         <v>330</v>
       </c>
-      <c r="D17" s="28"/>
-      <c r="E17" s="28"/>
-    </row>
-    <row r="18" spans="1:5" s="37" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A18" s="35" t="s">
+      <c r="D17" s="27"/>
+      <c r="E17" s="27"/>
+    </row>
+    <row r="18" spans="1:5" s="36" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A18" s="34" t="s">
         <v>319</v>
       </c>
-      <c r="B18" s="35" t="s">
+      <c r="B18" s="34" t="s">
         <v>335</v>
       </c>
-      <c r="C18" s="36" t="s">
+      <c r="C18" s="35" t="s">
         <v>337</v>
       </c>
-      <c r="D18" s="36"/>
-      <c r="E18" s="36"/>
-    </row>
-    <row r="19" spans="1:5" s="34" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A19" s="32" t="s">
+      <c r="D18" s="35"/>
+      <c r="E18" s="35"/>
+    </row>
+    <row r="19" spans="1:5" s="33" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A19" s="31" t="s">
         <v>328</v>
       </c>
-      <c r="B19" s="32" t="s">
+      <c r="B19" s="31" t="s">
         <v>329</v>
       </c>
-      <c r="C19" s="33" t="s">
+      <c r="C19" s="32" t="s">
         <v>340</v>
       </c>
-      <c r="D19" s="33"/>
-      <c r="E19" s="33"/>
-    </row>
-    <row r="20" spans="1:5" s="34" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A20" s="32"/>
-      <c r="B20" s="32"/>
-      <c r="C20" s="33"/>
-      <c r="D20" s="33"/>
-      <c r="E20" s="33"/>
+      <c r="D19" s="32"/>
+      <c r="E19" s="32"/>
+    </row>
+    <row r="20" spans="1:5" s="33" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A20" s="31"/>
+      <c r="B20" s="31"/>
+      <c r="C20" s="32"/>
+      <c r="D20" s="32"/>
+      <c r="E20" s="32"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>